<commit_message>
feat: Add detailed notebook header, automate library installation, create `Datalimpia.xlsx`, and modify `DireccionesUnicas.xlsx`.
</commit_message>
<xml_diff>
--- a/DireccionesUnicas.xlsx
+++ b/DireccionesUnicas.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2337,6 +2404,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>